<commit_message>
2021.10/12 seminar data update
</commit_message>
<xml_diff>
--- a/data/20211012/test_data.xlsx
+++ b/data/20211012/test_data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mailt\Desktop\RnD_Work\20210930\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{FC2AF845-81B3-46DA-827F-89BA6B2BD5A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35918619-4CF2-4652-90B7-7C1B2A4EA1D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41220" yWindow="555" windowWidth="31980" windowHeight="18690"/>
+    <workbookView xWindow="4755" yWindow="1335" windowWidth="28800" windowHeight="18120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="신호데이터" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="65">
   <si>
     <t>X</t>
   </si>
@@ -574,11 +574,38 @@
     "dist2": 1.0737045637133091,</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mac</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>dc:a6:32:d6:cc:04</t>
+  </si>
+  <si>
+    <t>AP 위치</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>시험 지점</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1353,7 +1380,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1411,10 +1438,19 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1479,16 +1515,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>243526</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>81601</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1511,7 +1547,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2743200" y="219075"/>
+          <a:off x="3952875" y="247650"/>
           <a:ext cx="10530526" cy="6610350"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1820,10 +1856,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -1839,20 +1875,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="20" t="s">
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
     </row>
     <row r="2" spans="1:13" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -3013,11 +3049,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -3293,135 +3329,233 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.75" customWidth="1"/>
+    <col min="3" max="3" width="14.125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C2" s="15" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B3" s="1">
         <v>187</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C3" s="3">
         <v>304</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
         <v>6</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B4" s="1">
         <v>347</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C4" s="3">
         <v>457</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
         <v>8</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B5" s="1">
         <v>528</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C5" s="3">
         <v>306</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
         <v>10</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B6" s="1">
         <v>703</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C6" s="3">
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
         <v>15</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B7" s="1">
         <v>878</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C7" s="3">
         <v>458</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
         <v>17</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B8" s="1">
         <v>1060</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C8" s="3">
         <v>301</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
         <v>19</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B9" s="1">
         <v>1202</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C9" s="3">
         <v>170</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
         <v>21</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B10" s="1">
         <v>1204</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C10" s="3">
         <v>459</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
         <v>22</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B11" s="1">
         <v>608</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C11" s="3">
         <v>567</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="4">
+    <row r="12" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="4">
         <v>27</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B12" s="5">
         <v>788</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C12" s="6">
         <v>776</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1200</v>
+      </c>
+      <c r="D16" s="3">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1175</v>
+      </c>
+      <c r="D17" s="3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>3</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="1">
+        <v>202</v>
+      </c>
+      <c r="D18" s="3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="1">
+        <v>185</v>
+      </c>
+      <c r="D19" s="3">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="4">
+        <v>5</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="5">
+        <v>699</v>
+      </c>
+      <c r="D20" s="6">
+        <v>817</v>
       </c>
     </row>
   </sheetData>

</xml_diff>